<commit_message>
edits to sql scripts for dimensions
</commit_message>
<xml_diff>
--- a/Jobupload.xlsx
+++ b/Jobupload.xlsx
@@ -1,43 +1,267 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/github/BI_Resume_tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EC32B44-0813-42CB-9CF9-21C9A0670008}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1797D8AB-29A6-F64C-8BFF-3361D07AF71A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35175" windowHeight="16313" xr2:uid="{2CF0A0A6-5B44-4F85-A182-BFCC5572270A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38840" windowHeight="31220" activeTab="3" xr2:uid="{2CF0A0A6-5B44-4F85-A182-BFCC5572270A}"/>
   </bookViews>
   <sheets>
-    <sheet name="JobData" sheetId="1" r:id="rId1"/>
+    <sheet name="person" sheetId="1" r:id="rId1"/>
+    <sheet name="WorkActivity" sheetId="2" r:id="rId2"/>
+    <sheet name="CompanyData" sheetId="3" r:id="rId3"/>
+    <sheet name="Skills" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{1E5EC405-86A8-954B-8DBB-28BB6D62F9F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use YYYYMMDD format. (4 digit year 2 digit month and 2 digit day) so January 1, 2018 is 20180101</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Zipcode</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Year Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Certified Solutions Architect – Associate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server 2000-2017 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSIS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSRS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS EC2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS S3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Cloudfront </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Route53 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS RDS (SQL Aurora) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Redshift </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Dynamo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS VPC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS ELB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Lambda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS IAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS GuardDuty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS CloudFormation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Config </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Trusted Advisor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS AutoScale </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS CloudWatch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Elastic MapReduce </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Chime </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS WorkSpaces </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS WorkDocs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Workmail </t>
+  </si>
+  <si>
+    <t>AWS SES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS SNS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS SQS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PowerShell </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python (2.x3.x) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS lightsail </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS Cognito </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystal Reports </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PowerBI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Azure </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS Office </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQLite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alteryx </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tableau </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agile </t>
+  </si>
+  <si>
+    <t>AWS CloudCommit</t>
+  </si>
+  <si>
+    <t>PowerQuery</t>
+  </si>
+  <si>
+    <t>PowerPivot</t>
+  </si>
+  <si>
+    <t>PowerView</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,8 +284,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,13 +601,493 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023A962F-08AE-4FF6-A99C-0CBB325A47E7}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="F1:I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68724771-A5B9-7146-90C1-467B9ECC717C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC352D3B-7E8E-2743-998A-E8F459625833}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D87BA2-6338-7648-8F05-7E8A23F9CD74}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>20181010</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>20070101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>20100101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>20100101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>20100101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>20171001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>20171001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>20180501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>20171001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>20151001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>20160101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29">
+        <v>20170101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>20100101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34">
+        <v>20130101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35">
+        <v>20170601</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37">
+        <v>20171001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>20150101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39">
+        <v>20150101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
+        <v>20070101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>20180101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42">
+        <v>20161101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43">
+        <v>20140101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44">
+        <v>20130401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45">
+        <v>20150101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47">
+        <v>20140601</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48">
+        <v>20140601</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49">
+        <v>20140601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7011AAE8-B6E1-404C-8A6D-3A5AD7F07EF8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding .gitignore for xlsx
</commit_message>
<xml_diff>
--- a/Jobupload.xlsx
+++ b/Jobupload.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/github/BI_Resume_tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1797D8AB-29A6-F64C-8BFF-3361D07AF71A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5857272B-54BE-0440-92E7-CA555DB40FE6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38840" windowHeight="31220" activeTab="3" xr2:uid="{2CF0A0A6-5B44-4F85-A182-BFCC5572270A}"/>
+    <workbookView xWindow="280" yWindow="1140" windowWidth="38840" windowHeight="31220" activeTab="2" xr2:uid="{2CF0A0A6-5B44-4F85-A182-BFCC5572270A}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
-    <sheet name="WorkActivity" sheetId="2" r:id="rId2"/>
-    <sheet name="CompanyData" sheetId="3" r:id="rId3"/>
-    <sheet name="Skills" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="CompanyData" sheetId="3" r:id="rId2"/>
+    <sheet name="Skills" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -62,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>FirstName</t>
   </si>
@@ -236,13 +234,88 @@
   </si>
   <si>
     <t>PowerView</t>
+  </si>
+  <si>
+    <t>CTO</t>
+  </si>
+  <si>
+    <t>Hotpathz Inc</t>
+  </si>
+  <si>
+    <t>VP of Engineering</t>
+  </si>
+  <si>
+    <t>Board Member Driver Rehabilitation Institute</t>
+  </si>
+  <si>
+    <t>President</t>
+  </si>
+  <si>
+    <t>Black Shell Consulting</t>
+  </si>
+  <si>
+    <t>Business Analytics Analyst IV</t>
+  </si>
+  <si>
+    <t>Beacon Hill Staffing</t>
+  </si>
+  <si>
+    <t>EMR/Soarian System Analyst</t>
+  </si>
+  <si>
+    <t>Arkansas Heart Hospital</t>
+  </si>
+  <si>
+    <t>Consultant</t>
+  </si>
+  <si>
+    <t>Health Data Specialists</t>
+  </si>
+  <si>
+    <t>Sr. Clinical Analyst</t>
+  </si>
+  <si>
+    <t>Southern New Hampshire Medical Center</t>
+  </si>
+  <si>
+    <t>03060</t>
+  </si>
+  <si>
+    <t>Clinical Consultant</t>
+  </si>
+  <si>
+    <t>Stoltenburg Consulting</t>
+  </si>
+  <si>
+    <t>15106</t>
+  </si>
+  <si>
+    <t>Implementation and Support Specialist</t>
+  </si>
+  <si>
+    <t>06105</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Huntley</t>
+  </si>
+  <si>
+    <t>chuntley@blackshellconsulting.com</t>
+  </si>
+  <si>
+    <t>JobStart</t>
+  </si>
+  <si>
+    <t>JobEnd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +336,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -281,14 +362,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -601,13 +686,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023A962F-08AE-4FF6-A99C-0CBB325A47E7}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="F1:I1"/>
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -624,6 +714,216 @@
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2">
+        <v>94947</v>
+      </c>
+      <c r="D2">
+        <v>4157746293</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{71DF1182-0CE5-C14A-ACCC-02F60A36B626}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC352D3B-7E8E-2743-998A-E8F459625833}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2">
+        <v>94947</v>
+      </c>
+      <c r="D2">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="2">
+        <v>94947</v>
+      </c>
+      <c r="D3">
+        <v>20170901</v>
+      </c>
+      <c r="E3">
+        <v>20180301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="2">
+        <v>94947</v>
+      </c>
+      <c r="D4">
+        <v>20170901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2">
+        <v>76244</v>
+      </c>
+      <c r="D5">
+        <v>20151101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="2">
+        <v>75254</v>
+      </c>
+      <c r="D6">
+        <v>20161101</v>
+      </c>
+      <c r="E6">
+        <v>20170301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="2">
+        <v>72211</v>
+      </c>
+      <c r="D7">
+        <v>20130901</v>
+      </c>
+      <c r="E7">
+        <v>20151101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="2">
+        <v>70070</v>
+      </c>
+      <c r="D8">
+        <v>20130901</v>
+      </c>
+      <c r="E8">
+        <v>20120201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9">
+        <v>20080301</v>
+      </c>
+      <c r="E9">
+        <v>20120601</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>20100701</v>
+      </c>
+      <c r="E10">
+        <v>20120201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11">
+        <v>20010101</v>
+      </c>
+      <c r="E11">
+        <v>20070601</v>
       </c>
     </row>
   </sheetData>
@@ -631,45 +931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68724771-A5B9-7146-90C1-467B9ECC717C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC352D3B-7E8E-2743-998A-E8F459625833}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22D87BA2-6338-7648-8F05-7E8A23F9CD74}">
   <dimension ref="A1:C49"/>
   <sheetViews>
@@ -1079,16 +1341,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7011AAE8-B6E1-404C-8A6D-3A5AD7F07EF8}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>